<commit_message>
rename to ISA.xlsx add assembler XCode project (because that's what I like)
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="128">
   <si>
     <t>D16 instruction set</t>
   </si>
@@ -376,6 +376,33 @@
   </si>
   <si>
     <t>RCL</t>
+  </si>
+  <si>
+    <t>LDCP</t>
+  </si>
+  <si>
+    <t>Cp-sel</t>
+  </si>
+  <si>
+    <t>CR=coprocessor register</t>
+  </si>
+  <si>
+    <t>CR-4</t>
+  </si>
+  <si>
+    <t>CR-3</t>
+  </si>
+  <si>
+    <t>CR-2</t>
+  </si>
+  <si>
+    <t>CR-1</t>
+  </si>
+  <si>
+    <t>CR-0</t>
+  </si>
+  <si>
+    <t>STCP</t>
   </si>
 </sst>
 </file>
@@ -424,8 +451,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -439,13 +476,23 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -849,22 +896,22 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1065,22 +1112,22 @@
         <v>114</v>
       </c>
       <c r="J12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" t="s">
         <v>60</v>
       </c>
-      <c r="K12" t="s">
+      <c r="N12" t="s">
         <v>60</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>60</v>
-      </c>
-      <c r="M12" t="s">
-        <v>113</v>
-      </c>
-      <c r="N12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O12" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1104,6 +1151,12 @@
       <c r="C14" t="s">
         <v>58</v>
       </c>
+      <c r="G14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
@@ -1115,6 +1168,33 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
@@ -1126,6 +1206,30 @@
       <c r="C16" t="s">
         <v>58</v>
       </c>
+      <c r="H16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K16" t="s">
+        <v>125</v>
+      </c>
+      <c r="L16" t="s">
+        <v>126</v>
+      </c>
+      <c r="M16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -1137,9 +1241,6 @@
       <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="G17" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
@@ -1151,12 +1252,6 @@
       <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
@@ -1172,7 +1267,7 @@
         <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1186,7 +1281,10 @@
         <v>63</v>
       </c>
       <c r="G20" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1203,7 +1301,7 @@
         <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1217,7 +1315,7 @@
         <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1234,7 +1332,7 @@
         <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1248,7 +1346,7 @@
         <v>63</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1265,7 +1363,7 @@
         <v>73</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1279,7 +1377,7 @@
         <v>63</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1293,7 +1391,7 @@
         <v>63</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1307,7 +1405,7 @@
         <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1324,7 +1422,7 @@
         <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1338,7 +1436,7 @@
         <v>63</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1355,7 +1453,7 @@
         <v>73</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1369,7 +1467,7 @@
         <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1386,7 +1484,7 @@
         <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1400,7 +1498,7 @@
         <v>63</v>
       </c>
       <c r="G34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1417,7 +1515,7 @@
         <v>73</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1431,7 +1529,7 @@
         <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1448,7 +1546,7 @@
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1462,7 +1560,7 @@
         <v>82</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1476,7 +1574,7 @@
         <v>108</v>
       </c>
       <c r="G39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1490,7 +1588,7 @@
         <v>110</v>
       </c>
       <c r="G40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1504,7 +1602,7 @@
         <v>110</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1518,7 +1616,7 @@
         <v>110</v>
       </c>
       <c r="G42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1531,15 +1629,33 @@
       <c r="C43" t="s">
         <v>110</v>
       </c>
+      <c r="G43" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>91</v>
       </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:7">

</xml_diff>

<commit_message>
major restructuring of the ISA moved immediate instructions to 128+the non immediate instruction
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="15940" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
   <si>
     <t>D16 instruction set</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>NEG</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>LD</t>
@@ -328,7 +325,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +349,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -370,7 +374,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,14 +404,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -422,6 +471,28 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -436,6 +507,28 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -765,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -866,17 +959,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4:B58" si="0">DEC2HEX(A4,2)</f>
+        <f t="shared" ref="B4:B67" si="0">DEC2HEX(A4,2)</f>
         <v>01</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -888,7 +978,7 @@
         <v>02</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
@@ -903,16 +993,13 @@
         <v>03</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -924,13 +1011,13 @@
         <v>04</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7">
         <v>7</v>
@@ -966,28 +1053,25 @@
         <v>05</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N8" t="s">
         <v>52</v>
@@ -1008,10 +1092,10 @@
         <v>06</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1023,13 +1107,13 @@
         <v>07</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1041,13 +1125,13 @@
         <v>08</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11">
         <v>7</v>
@@ -1083,7 +1167,7 @@
         <v>09</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -1092,16 +1176,16 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N12" t="s">
         <v>48</v>
@@ -1122,7 +1206,7 @@
         <v>0A</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -1137,16 +1221,16 @@
         <v>0B</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="H14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" t="s">
         <v>89</v>
-      </c>
-      <c r="I14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1158,13 +1242,13 @@
         <v>0C</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I15">
         <v>7</v>
@@ -1200,25 +1284,25 @@
         <v>0D</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" t="s">
         <v>91</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>92</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>93</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>94</v>
-      </c>
-      <c r="M16" t="s">
-        <v>95</v>
       </c>
       <c r="N16" t="s">
         <v>48</v>
@@ -1239,10 +1323,10 @@
         <v>0E</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1254,10 +1338,10 @@
         <v>0F</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1269,16 +1353,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
-        <v>61</v>
-      </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1290,7 +1371,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -1299,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1311,13 +1392,10 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
         <v>51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
       </c>
       <c r="H21" t="s">
         <v>3</v>
@@ -1332,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
         <v>51</v>
@@ -1350,13 +1428,10 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>61</v>
       </c>
       <c r="H23" t="s">
         <v>5</v>
@@ -1371,7 +1446,7 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -1389,13 +1464,10 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H25" t="s">
         <v>7</v>
@@ -1410,10 +1482,10 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="H26" t="s">
         <v>8</v>
@@ -1428,10 +1500,10 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s">
         <v>9</v>
@@ -1446,7 +1518,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
         <v>51</v>
@@ -1464,13 +1536,10 @@
         <v>1A</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
-      </c>
-      <c r="E29" t="s">
-        <v>61</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -1485,7 +1554,7 @@
         <v>1B</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
         <v>51</v>
@@ -1503,13 +1572,10 @@
         <v>1C</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
         <v>51</v>
-      </c>
-      <c r="E31" t="s">
-        <v>61</v>
       </c>
       <c r="H31" t="s">
         <v>13</v>
@@ -1524,10 +1590,10 @@
         <v>1D</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s">
         <v>14</v>
@@ -1542,13 +1608,10 @@
         <v>1E</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -1562,12 +1625,6 @@
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" t="s">
-        <v>51</v>
-      </c>
       <c r="H34" t="s">
         <v>16</v>
       </c>
@@ -1580,15 +1637,6 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" t="s">
-        <v>61</v>
-      </c>
       <c r="H35" t="s">
         <v>17</v>
       </c>
@@ -1601,12 +1649,6 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" t="s">
-        <v>70</v>
-      </c>
       <c r="H36" t="s">
         <v>18</v>
       </c>
@@ -1619,15 +1661,6 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" t="s">
-        <v>61</v>
-      </c>
       <c r="H37" t="s">
         <v>19</v>
       </c>
@@ -1640,12 +1673,6 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" t="s">
-        <v>70</v>
-      </c>
       <c r="H38" t="s">
         <v>20</v>
       </c>
@@ -1658,12 +1685,6 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C39" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" t="s">
-        <v>77</v>
-      </c>
       <c r="H39" t="s">
         <v>21</v>
       </c>
@@ -1676,12 +1697,6 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" t="s">
-        <v>79</v>
-      </c>
       <c r="H40" t="s">
         <v>22</v>
       </c>
@@ -1694,12 +1709,6 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" t="s">
-        <v>51</v>
-      </c>
       <c r="H41" t="s">
         <v>23</v>
       </c>
@@ -1712,12 +1721,6 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" t="s">
-        <v>79</v>
-      </c>
       <c r="H42" t="s">
         <v>24</v>
       </c>
@@ -1730,12 +1733,6 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" t="s">
-        <v>51</v>
-      </c>
       <c r="H43" t="s">
         <v>25</v>
       </c>
@@ -1748,12 +1745,6 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>79</v>
-      </c>
       <c r="H44" t="s">
         <v>26</v>
       </c>
@@ -1766,12 +1757,6 @@
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
-      <c r="C45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
@@ -1781,12 +1766,6 @@
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
-      <c r="C46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
@@ -1796,12 +1775,6 @@
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
-      <c r="C47" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
@@ -1811,14 +1784,8 @@
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-      <c r="C48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1826,14 +1793,8 @@
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1842,7 +1803,7 @@
         <v>2F</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1851,7 +1812,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1860,7 +1821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1869,7 +1830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1878,7 +1839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>52</v>
       </c>
@@ -1887,7 +1848,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>53</v>
       </c>
@@ -1896,7 +1857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>54</v>
       </c>
@@ -1905,13 +1866,1949 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3D</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3E</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3F</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f t="shared" ref="B68:B131" si="1">DEC2HEX(A68,2)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4B</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4C</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4D</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4E</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5B</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5C</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5D</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5E</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>5F</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6A</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6B</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6C</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6D</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6E</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>6F</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>115</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123">
+        <v>120</v>
+      </c>
+      <c r="B123" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124">
+        <v>121</v>
+      </c>
+      <c r="B124" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125">
+        <v>122</v>
+      </c>
+      <c r="B125" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7A</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126">
+        <v>123</v>
+      </c>
+      <c r="B126" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7B</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127">
+        <v>124</v>
+      </c>
+      <c r="B127" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7C</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128">
+        <v>125</v>
+      </c>
+      <c r="B128" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7D</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>126</v>
+      </c>
+      <c r="B129" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>127</v>
+      </c>
+      <c r="B130" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7F</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>128</v>
+      </c>
+      <c r="B131" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>129</v>
+      </c>
+      <c r="B132" s="1" t="str">
+        <f t="shared" ref="B132:B195" si="2">DEC2HEX(A132,2)</f>
+        <v>81</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>130</v>
+      </c>
+      <c r="B133" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="B134" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>132</v>
+      </c>
+      <c r="B135" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>133</v>
+      </c>
+      <c r="B136" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>134</v>
+      </c>
+      <c r="B137" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>135</v>
+      </c>
+      <c r="B138" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139">
+        <v>136</v>
+      </c>
+      <c r="B139" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140">
+        <v>137</v>
+      </c>
+      <c r="B140" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141">
+        <v>138</v>
+      </c>
+      <c r="B141" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8A</v>
+      </c>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142">
+        <v>139</v>
+      </c>
+      <c r="B142" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8B</v>
+      </c>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143">
+        <v>140</v>
+      </c>
+      <c r="B143" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8C</v>
+      </c>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144">
+        <v>141</v>
+      </c>
+      <c r="B144" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8D</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145">
+        <v>142</v>
+      </c>
+      <c r="B145" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8E</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146">
+        <v>143</v>
+      </c>
+      <c r="B146" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>8F</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147">
+        <v>144</v>
+      </c>
+      <c r="B147" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148">
+        <v>145</v>
+      </c>
+      <c r="B148" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149">
+        <v>146</v>
+      </c>
+      <c r="B149" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150">
+        <v>147</v>
+      </c>
+      <c r="B150" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151">
+        <v>148</v>
+      </c>
+      <c r="B151" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152">
+        <v>149</v>
+      </c>
+      <c r="B152" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153">
+        <v>150</v>
+      </c>
+      <c r="B153" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154">
+        <v>151</v>
+      </c>
+      <c r="B154" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155">
+        <v>152</v>
+      </c>
+      <c r="B155" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156">
+        <v>153</v>
+      </c>
+      <c r="B156" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157">
+        <v>154</v>
+      </c>
+      <c r="B157" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9A</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158">
+        <v>155</v>
+      </c>
+      <c r="B158" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9B</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159">
+        <v>156</v>
+      </c>
+      <c r="B159" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9C</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160">
+        <v>157</v>
+      </c>
+      <c r="B160" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9D</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161">
+        <v>158</v>
+      </c>
+      <c r="B161" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9E</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162">
+        <v>159</v>
+      </c>
+      <c r="B162" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>9F</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A0</v>
+      </c>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164">
+        <v>161</v>
+      </c>
+      <c r="B164" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165">
+        <v>162</v>
+      </c>
+      <c r="B165" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A2</v>
+      </c>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A3</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A5</v>
+      </c>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A6</v>
+      </c>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A7</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172">
+        <v>169</v>
+      </c>
+      <c r="B172" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>A9</v>
+      </c>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173">
+        <v>170</v>
+      </c>
+      <c r="B173" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AA</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174">
+        <v>171</v>
+      </c>
+      <c r="B174" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AB</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175">
+        <v>172</v>
+      </c>
+      <c r="B175" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AC</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176">
+        <v>173</v>
+      </c>
+      <c r="B176" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AD</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177">
+        <v>174</v>
+      </c>
+      <c r="B177" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AE</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178">
+        <v>175</v>
+      </c>
+      <c r="B178" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AF</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179">
+        <v>176</v>
+      </c>
+      <c r="B179" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180">
+        <v>177</v>
+      </c>
+      <c r="B180" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181">
+        <v>178</v>
+      </c>
+      <c r="B181" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182">
+        <v>179</v>
+      </c>
+      <c r="B182" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183">
+        <v>180</v>
+      </c>
+      <c r="B183" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184">
+        <v>181</v>
+      </c>
+      <c r="B184" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185">
+        <v>182</v>
+      </c>
+      <c r="B185" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186">
+        <v>183</v>
+      </c>
+      <c r="B186" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187">
+        <v>184</v>
+      </c>
+      <c r="B187" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188">
+        <v>185</v>
+      </c>
+      <c r="B188" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>B9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189">
+        <v>186</v>
+      </c>
+      <c r="B189" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BA</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190">
+        <v>187</v>
+      </c>
+      <c r="B190" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BB</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191">
+        <v>188</v>
+      </c>
+      <c r="B191" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BC</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192">
+        <v>189</v>
+      </c>
+      <c r="B192" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BD</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193">
+        <v>190</v>
+      </c>
+      <c r="B193" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BE</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194">
+        <v>191</v>
+      </c>
+      <c r="B194" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>BF</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195">
+        <v>192</v>
+      </c>
+      <c r="B195" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>C0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196">
+        <v>193</v>
+      </c>
+      <c r="B196" s="1" t="str">
+        <f t="shared" ref="B196:B258" si="3">DEC2HEX(A196,2)</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197">
+        <v>194</v>
+      </c>
+      <c r="B197" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198">
+        <v>195</v>
+      </c>
+      <c r="B198" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199">
+        <v>196</v>
+      </c>
+      <c r="B199" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200">
+        <v>197</v>
+      </c>
+      <c r="B200" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201">
+        <v>198</v>
+      </c>
+      <c r="B201" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202">
+        <v>199</v>
+      </c>
+      <c r="B202" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203">
+        <v>200</v>
+      </c>
+      <c r="B203" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204">
+        <v>201</v>
+      </c>
+      <c r="B204" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>C9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205">
+        <v>202</v>
+      </c>
+      <c r="B205" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206">
+        <v>203</v>
+      </c>
+      <c r="B206" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CB</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207">
+        <v>204</v>
+      </c>
+      <c r="B207" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CC</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208">
+        <v>205</v>
+      </c>
+      <c r="B208" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CD</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209">
+        <v>206</v>
+      </c>
+      <c r="B209" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CE</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210">
+        <v>207</v>
+      </c>
+      <c r="B210" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CF</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211">
+        <v>208</v>
+      </c>
+      <c r="B211" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212">
+        <v>209</v>
+      </c>
+      <c r="B212" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213">
+        <v>210</v>
+      </c>
+      <c r="B213" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214">
+        <v>211</v>
+      </c>
+      <c r="B214" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215">
+        <v>212</v>
+      </c>
+      <c r="B215" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216">
+        <v>213</v>
+      </c>
+      <c r="B216" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217">
+        <v>214</v>
+      </c>
+      <c r="B217" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D6</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218">
+        <v>215</v>
+      </c>
+      <c r="B218" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219">
+        <v>216</v>
+      </c>
+      <c r="B219" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220">
+        <v>217</v>
+      </c>
+      <c r="B220" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>D9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221">
+        <v>218</v>
+      </c>
+      <c r="B221" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DA</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222">
+        <v>219</v>
+      </c>
+      <c r="B222" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DB</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223">
+        <v>220</v>
+      </c>
+      <c r="B223" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DC</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224">
+        <v>221</v>
+      </c>
+      <c r="B224" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DD</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225">
+        <v>222</v>
+      </c>
+      <c r="B225" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226">
+        <v>223</v>
+      </c>
+      <c r="B226" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DF</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227">
+        <v>224</v>
+      </c>
+      <c r="B227" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228">
+        <v>225</v>
+      </c>
+      <c r="B228" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229">
+        <v>226</v>
+      </c>
+      <c r="B229" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230">
+        <v>227</v>
+      </c>
+      <c r="B230" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231">
+        <v>228</v>
+      </c>
+      <c r="B231" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232">
+        <v>229</v>
+      </c>
+      <c r="B232" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233">
+        <v>230</v>
+      </c>
+      <c r="B233" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234">
+        <v>231</v>
+      </c>
+      <c r="B234" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235">
+        <v>232</v>
+      </c>
+      <c r="B235" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236">
+        <v>233</v>
+      </c>
+      <c r="B236" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>E9</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237">
+        <v>234</v>
+      </c>
+      <c r="B237" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>EA</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238">
+        <v>235</v>
+      </c>
+      <c r="B238" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>EB</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239">
+        <v>236</v>
+      </c>
+      <c r="B239" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>EC</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240">
+        <v>237</v>
+      </c>
+      <c r="B240" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ED</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241">
+        <v>238</v>
+      </c>
+      <c r="B241" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>EE</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242">
+        <v>239</v>
+      </c>
+      <c r="B242" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>EF</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243">
+        <v>240</v>
+      </c>
+      <c r="B243" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244">
+        <v>241</v>
+      </c>
+      <c r="B244" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245">
+        <v>242</v>
+      </c>
+      <c r="B245" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246">
+        <v>243</v>
+      </c>
+      <c r="B246" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247">
+        <v>244</v>
+      </c>
+      <c r="B247" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248">
+        <v>245</v>
+      </c>
+      <c r="B248" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249">
+        <v>246</v>
+      </c>
+      <c r="B249" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250">
+        <v>247</v>
+      </c>
+      <c r="B250" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251">
+        <v>248</v>
+      </c>
+      <c r="B251" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252">
+        <v>249</v>
+      </c>
+      <c r="B252" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>F9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253">
+        <v>250</v>
+      </c>
+      <c r="B253" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FA</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254">
+        <v>251</v>
+      </c>
+      <c r="B254" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FB</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255">
+        <v>252</v>
+      </c>
+      <c r="B255" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FC</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256">
+        <v>253</v>
+      </c>
+      <c r="B256" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FD</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257">
+        <v>254</v>
+      </c>
+      <c r="B257" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FE</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258">
+        <v>255</v>
+      </c>
+      <c r="B258" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>FF</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add add with carry and subtract with borrow opcodes And some very ugly typecasts in alu.vhd
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
     <t>D16 instruction set</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>Sign</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>SBB</t>
   </si>
 </sst>
 </file>
@@ -449,8 +455,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -555,7 +565,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -604,6 +614,8 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -652,6 +664,8 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -983,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:N35"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,8 +1198,8 @@
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="I8" t="s">
-        <v>71</v>
+      <c r="I8">
+        <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>71</v>
@@ -1883,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1916,7 +1930,7 @@
         <v>14</v>
       </c>
       <c r="J32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -1949,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="J33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -1972,11 +1986,17 @@
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
       <c r="H34" t="s">
         <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -1999,11 +2019,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="C35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
       <c r="H35" t="s">
         <v>17</v>
       </c>
       <c r="J35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -2015,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="N35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2029,6 +2055,21 @@
       <c r="H36" t="s">
         <v>18</v>
       </c>
+      <c r="J36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37">
@@ -3309,6 +3350,12 @@
         <f t="shared" si="2"/>
         <v>9F</v>
       </c>
+      <c r="C162" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163">
@@ -3318,8 +3365,12 @@
         <f t="shared" si="2"/>
         <v>A0</v>
       </c>
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
+      <c r="C163" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164">

</xml_diff>

<commit_message>
Add new encoding for Loads and Stores Now allows for bytewise stores, as well as offsets
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="134">
   <si>
     <t>D16 instruction set</t>
   </si>
@@ -400,6 +400,27 @@
   </si>
   <si>
     <t>SBB</t>
+  </si>
+  <si>
+    <t>reg-sel-disp</t>
+  </si>
+  <si>
+    <t>Reg-sel-disp</t>
+  </si>
+  <si>
+    <t>Byte flag</t>
+  </si>
+  <si>
+    <t>*Byte flag if mem instruction</t>
+  </si>
+  <si>
+    <t>0*</t>
+  </si>
+  <si>
+    <t>offset flag</t>
+  </si>
+  <si>
+    <t>When the offset flag is set, the address is calculated as the signed addition of rS+the immediate</t>
   </si>
 </sst>
 </file>
@@ -455,8 +476,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -565,7 +594,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -616,6 +645,10 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -666,6 +699,10 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -997,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1010,7 +1047,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1024,31 +1061,31 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>3</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0</v>
       </c>
     </row>
@@ -1069,8 +1106,8 @@
       <c r="H3" t="s">
         <v>46</v>
       </c>
-      <c r="I3">
-        <v>0</v>
+      <c r="I3" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1108,6 +1145,9 @@
       <c r="D4" t="s">
         <v>51</v>
       </c>
+      <c r="I4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
@@ -1483,6 +1523,33 @@
       <c r="D18" t="s">
         <v>51</v>
       </c>
+      <c r="H18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19">
@@ -1498,11 +1565,29 @@
       <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="s">
-        <v>76</v>
+      <c r="I19" t="s">
+        <v>129</v>
       </c>
       <c r="J19" t="s">
-        <v>100</v>
+        <v>132</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1519,26 +1604,8 @@
       <c r="D20" t="s">
         <v>51</v>
       </c>
-      <c r="H20" t="s">
-        <v>1</v>
-      </c>
       <c r="I20" t="s">
-        <v>77</v>
-      </c>
-      <c r="J20" t="s">
-        <v>105</v>
-      </c>
-      <c r="K20" t="s">
-        <v>101</v>
-      </c>
-      <c r="L20" t="s">
-        <v>102</v>
-      </c>
-      <c r="M20" t="s">
-        <v>103</v>
-      </c>
-      <c r="N20" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1555,24 +1622,6 @@
       <c r="D21" t="s">
         <v>51</v>
       </c>
-      <c r="H21" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" t="s">
-        <v>120</v>
-      </c>
-      <c r="K21" t="s">
-        <v>124</v>
-      </c>
-      <c r="L21" t="s">
-        <v>123</v>
-      </c>
-      <c r="M21" t="s">
-        <v>121</v>
-      </c>
-      <c r="N21" t="s">
-        <v>122</v>
-      </c>
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16">
@@ -1589,24 +1638,6 @@
       <c r="D22" t="s">
         <v>51</v>
       </c>
-      <c r="H22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
-        <v>106</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16">
@@ -1623,24 +1654,6 @@
       <c r="D23" t="s">
         <v>51</v>
       </c>
-      <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" t="s">
-        <v>107</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16">
@@ -1657,24 +1670,6 @@
       <c r="D24" t="s">
         <v>51</v>
       </c>
-      <c r="H24" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" t="s">
-        <v>108</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16">
@@ -1691,24 +1686,6 @@
       <c r="D25" t="s">
         <v>69</v>
       </c>
-      <c r="H25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" t="s">
-        <v>109</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16">
@@ -1725,24 +1702,6 @@
       <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="H26" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26" t="s">
-        <v>110</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16">
@@ -1759,24 +1718,6 @@
       <c r="D27" t="s">
         <v>76</v>
       </c>
-      <c r="H27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" t="s">
-        <v>111</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16">
@@ -1793,24 +1734,6 @@
       <c r="D28" t="s">
         <v>51</v>
       </c>
-      <c r="H28" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" t="s">
-        <v>112</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16">
@@ -1827,24 +1750,6 @@
       <c r="D29" t="s">
         <v>51</v>
       </c>
-      <c r="H29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J29" t="s">
-        <v>113</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
@@ -1860,24 +1765,6 @@
       <c r="D30" t="s">
         <v>51</v>
       </c>
-      <c r="H30" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" t="s">
-        <v>114</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
@@ -1893,24 +1780,6 @@
       <c r="D31" t="s">
         <v>51</v>
       </c>
-      <c r="H31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" t="s">
-        <v>71</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
@@ -1926,24 +1795,6 @@
       <c r="D32" t="s">
         <v>88</v>
       </c>
-      <c r="H32" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" t="s">
-        <v>115</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33">
@@ -1959,24 +1810,6 @@
       <c r="D33" t="s">
         <v>88</v>
       </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34">
@@ -1993,22 +1826,10 @@
         <v>51</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="J34" t="s">
-        <v>117</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2026,22 +1847,25 @@
         <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>77</v>
       </c>
       <c r="J35" t="s">
-        <v>118</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="K35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L35" t="s">
+        <v>102</v>
+      </c>
+      <c r="M35" t="s">
+        <v>103</v>
+      </c>
+      <c r="N35" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2053,22 +1877,22 @@
         <v>21</v>
       </c>
       <c r="H36" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J36" t="s">
-        <v>119</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="K36" t="s">
+        <v>124</v>
+      </c>
+      <c r="L36" t="s">
+        <v>123</v>
+      </c>
+      <c r="M36" t="s">
+        <v>121</v>
+      </c>
+      <c r="N36" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2080,7 +1904,22 @@
         <v>22</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="J37" t="s">
+        <v>106</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2092,7 +1931,22 @@
         <v>23</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2104,7 +1958,22 @@
         <v>24</v>
       </c>
       <c r="H39" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="J39" t="s">
+        <v>108</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2116,7 +1985,22 @@
         <v>25</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>109</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2128,7 +2012,22 @@
         <v>26</v>
       </c>
       <c r="H41" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="J41" t="s">
+        <v>110</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2140,7 +2039,22 @@
         <v>27</v>
       </c>
       <c r="H42" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="J42" t="s">
+        <v>111</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2152,7 +2066,22 @@
         <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="J43" t="s">
+        <v>112</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2164,7 +2093,22 @@
         <v>29</v>
       </c>
       <c r="H44" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>113</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2175,6 +2119,24 @@
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
+      <c r="H45" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" t="s">
+        <v>114</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46">
@@ -2184,6 +2146,24 @@
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" t="s">
+        <v>71</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:14">
       <c r="A47">
@@ -2193,6 +2173,24 @@
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" t="s">
+        <v>115</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48">
@@ -2202,8 +2200,26 @@
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" t="s">
+        <v>116</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49">
         <v>46</v>
       </c>
@@ -2211,8 +2227,26 @@
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="H49" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" t="s">
+        <v>117</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50">
         <v>47</v>
       </c>
@@ -2220,8 +2254,26 @@
         <f t="shared" si="0"/>
         <v>2F</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="H50" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" t="s">
+        <v>118</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51">
         <v>48</v>
       </c>
@@ -2229,8 +2281,26 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="H51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" t="s">
+        <v>119</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52">
         <v>49</v>
       </c>
@@ -2238,8 +2308,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="H52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2247,8 +2320,11 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54">
         <v>51</v>
       </c>
@@ -2256,8 +2332,11 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55">
         <v>52</v>
       </c>
@@ -2265,8 +2344,11 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="H55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2274,8 +2356,11 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57">
         <v>54</v>
       </c>
@@ -2283,8 +2368,11 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="H57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58">
         <v>55</v>
       </c>
@@ -2292,8 +2380,11 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59">
         <v>56</v>
       </c>
@@ -2301,8 +2392,11 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="H59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60">
         <v>57</v>
       </c>
@@ -2311,7 +2405,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:14">
       <c r="A61">
         <v>58</v>
       </c>
@@ -2320,7 +2414,7 @@
         <v>3A</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:14">
       <c r="A62">
         <v>59</v>
       </c>
@@ -2329,7 +2423,7 @@
         <v>3B</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:14">
       <c r="A63">
         <v>60</v>
       </c>
@@ -2338,7 +2432,7 @@
         <v>3C</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:14">
       <c r="A64">
         <v>61</v>
       </c>
@@ -3188,7 +3282,7 @@
         <v>62</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3203,7 +3297,7 @@
         <v>64</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
     </row>
     <row r="152" spans="1:4">

</xml_diff>

<commit_message>
Remove special shift selector
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1440" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,8 +476,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,7 +610,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -649,6 +665,14 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -703,6 +727,14 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1034,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3368,7 +3400,7 @@
         <v>96</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3383,7 +3415,7 @@
         <v>97</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3398,7 +3430,7 @@
         <v>98</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3413,7 +3445,7 @@
         <v>99</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="160" spans="1:4">

</xml_diff>